<commit_message>
revise ND_HOWLONG Never returned name to Not returned
</commit_message>
<xml_diff>
--- a/Data_Dictionary.xlsx
+++ b/Data_Dictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolepaul/Code/us-household-pulse-disasters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolepaul/Code/dash-ushh-displacement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C0FCF00-B6B4-9242-B4BF-32771844D371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDA80B7-A253-0142-948B-1AA6AFED652E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10200" yWindow="500" windowWidth="25580" windowHeight="20720" xr2:uid="{91BCF11A-B2C4-4646-8B3D-9FD1FC987647}"/>
   </bookViews>
@@ -613,7 +613,7 @@
 2) Less than a month
 3) One to six months
 4) More than six months
-5) Never returned
+5) Not returned
 -99) Not selected
 -88) Missing/DNR</t>
   </si>
@@ -674,7 +674,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -686,7 +686,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -718,9 +717,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -758,7 +757,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -864,7 +863,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1006,7 +1005,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1266,7 +1265,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="119" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+      <c r="A18" t="s">
         <v>132</v>
       </c>
       <c r="B18" t="s">
@@ -1294,7 +1293,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="102" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
+      <c r="A20" t="s">
         <v>133</v>
       </c>
       <c r="B20" t="s">

</xml_diff>